<commit_message>
PCB is done except for DRC, BOM is done
</commit_message>
<xml_diff>
--- a/battery_monitoring_board/V2_2018_2019/Hotswap_BOM.xlsx
+++ b/battery_monitoring_board/V2_2018_2019/Hotswap_BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -99,48 +99,9 @@
     <t>http://www.yageo.com/documents/recent/PYu-RC_Group_51_RoHS_L_9.pdf</t>
   </si>
   <si>
-    <t>RES SMD 12.4K OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
-    <t>RC1206FR-0712K4L</t>
-  </si>
-  <si>
-    <t>RES 9.09K OHM 1% 1/2W 1206</t>
-  </si>
-  <si>
-    <t>RNCP1206FTD9K09</t>
-  </si>
-  <si>
     <t>https://www.seielect.com/Catalog/SEI-rncp.pdf</t>
   </si>
   <si>
-    <t>RES SMD 158K OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
-    <t>RC1206FR-07158KL</t>
-  </si>
-  <si>
-    <t>RES SMD 2.32K OHM 1% 1/4W 1206</t>
-  </si>
-  <si>
-    <t>RC1206FR-072K32L</t>
-  </si>
-  <si>
-    <t>CAP CER 1206 1NF 25V X7R 5%</t>
-  </si>
-  <si>
-    <t>399-19000-1-ND</t>
-  </si>
-  <si>
-    <t>https://content.kemet.com/datasheets/KEM_C1090_X7R_ESD.pdf</t>
-  </si>
-  <si>
-    <t>CAP CER 1206 0.1UF 25V X7R 5%</t>
-  </si>
-  <si>
-    <t>399-19001-1-ND</t>
-  </si>
-  <si>
     <t>C1,C2,C4,C5,C6</t>
   </si>
   <si>
@@ -163,6 +124,51 @@
   </si>
   <si>
     <t>http://www.kingbrightusa.com/images/catalog/SPEC/APTD2012LQBC-D.pdf</t>
+  </si>
+  <si>
+    <t>RES 12.4K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD12K4</t>
+  </si>
+  <si>
+    <t>RES 9.09K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD9K09</t>
+  </si>
+  <si>
+    <t>RES SMD 158K OHM 0.5% 1/4W 0805</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ERJ-PB6D1583V </t>
+  </si>
+  <si>
+    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDM0000/AOA0000C328.pdf</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 25V X7R 0805</t>
+  </si>
+  <si>
+    <t>VJ0805Y102JXXPW1BC</t>
+  </si>
+  <si>
+    <t>https://www.vishay.com/docs/28548/vjw1bcbascomseries.pdf</t>
+  </si>
+  <si>
+    <t>http://datasheets.avx.com/AutoMLCC.pdf</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0805</t>
+  </si>
+  <si>
+    <t>08055C104J4T2A</t>
+  </si>
+  <si>
+    <t>RES 2.32K OHM 1% 1/4W 0805</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD2K32</t>
   </si>
 </sst>
 </file>
@@ -516,7 +522,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -527,7 +533,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,13 +631,13 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E5" s="1">
         <v>0.93</v>
@@ -673,23 +679,23 @@
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F7" s="1">
         <v>2</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -697,95 +703,95 @@
         <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E9" s="1">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="1">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E11" s="1">
-        <v>0.41</v>
+        <v>0.27</v>
       </c>
       <c r="F11" s="1">
         <v>5</v>
       </c>
       <c r="G11" s="1">
         <f>F11*E11</f>
-        <v>2.0499999999999998</v>
+        <v>1.35</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -793,37 +799,37 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1">
-        <v>0.4</v>
+        <v>0.34</v>
       </c>
       <c r="F12" s="1">
         <v>1</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" ref="G12:G13" si="1">F12*E12</f>
-        <v>0.4</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1">
         <v>1.94</v>
@@ -847,7 +853,7 @@
       </c>
       <c r="G16" s="4">
         <f>SUM(G3:G12)</f>
-        <v>29.610000000000003</v>
+        <v>28.650000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -856,8 +862,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D9" r:id="rId2"/>
+    <hyperlink ref="D12" r:id="rId3"/>
+    <hyperlink ref="D10" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>